<commit_message>
updates made for reclamation facility analysis
</commit_message>
<xml_diff>
--- a/output/Allocation Rule/facility_data/allocation_rule_facility_demographics_3mi.xlsx
+++ b/output/Allocation Rule/facility_data/allocation_rule_facility_demographics_3mi.xlsx
@@ -530,52 +530,52 @@
         <v>96067</v>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" t="n">
-        <v>79.1835308238153</v>
+        <v>93.6022758618435</v>
       </c>
       <c r="F2" t="n">
-        <v>13669</v>
+        <v>14738</v>
       </c>
       <c r="G2" t="n">
-        <v>172.624280046488</v>
+        <v>157.453436514228</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1</v>
+        <v>0.091</v>
       </c>
       <c r="J2" t="n">
-        <v>7231</v>
+        <v>7333</v>
       </c>
       <c r="K2" t="n">
-        <v>5305</v>
+        <v>5746</v>
       </c>
       <c r="L2" t="n">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="M2" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>1979</v>
+        <v>2364</v>
       </c>
       <c r="O2" t="n">
-        <v>42.2702</v>
+        <v>51.4409</v>
       </c>
       <c r="P2" t="n">
-        <v>10.4039757209588</v>
+        <v>8.05941363323641</v>
       </c>
       <c r="Q2" t="n">
-        <v>17.2954604417089</v>
+        <v>14.6877224931919</v>
       </c>
       <c r="R2" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="S2" t="n">
-        <v>0.53</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="3">
@@ -592,13 +592,13 @@
         <v>3</v>
       </c>
       <c r="E3" t="n">
-        <v>103.612502034919</v>
+        <v>96.6011004628816</v>
       </c>
       <c r="F3" t="n">
-        <v>4731</v>
+        <v>2871</v>
       </c>
       <c r="G3" t="n">
-        <v>45.6605130373706</v>
+        <v>29.7201583236949</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
@@ -607,34 +607,34 @@
         <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>4443</v>
+        <v>2626</v>
       </c>
       <c r="K3" t="n">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="L3" t="n">
-        <v>169</v>
+        <v>216</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="O3" t="n">
-        <v>71.0786666666667</v>
+        <v>89.3893333333333</v>
       </c>
       <c r="P3" t="n">
-        <v>4.7675821045964</v>
+        <v>2.97911209099006</v>
       </c>
       <c r="Q3" t="n">
-        <v>6.92743033168565</v>
-      </c>
-      <c r="R3" t="n">
-        <v>50</v>
-      </c>
-      <c r="S3" t="n">
-        <v>0.5</v>
+        <v>5.20403060332032</v>
+      </c>
+      <c r="R3" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S3" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="4">
@@ -648,49 +648,49 @@
         <v>2619</v>
       </c>
       <c r="D4" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E4" t="n">
-        <v>75.1709513066939</v>
+        <v>74.4371247489178</v>
       </c>
       <c r="F4" t="n">
-        <v>24988</v>
+        <v>25972</v>
       </c>
       <c r="G4" t="n">
-        <v>332.415641489625</v>
+        <v>348.91191844937</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.48</v>
+        <v>0.45</v>
       </c>
       <c r="J4" t="n">
-        <v>17406</v>
+        <v>17965</v>
       </c>
       <c r="K4" t="n">
-        <v>5094</v>
+        <v>4775</v>
       </c>
       <c r="L4" t="n">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="M4" t="n">
-        <v>303</v>
+        <v>207</v>
       </c>
       <c r="N4" t="n">
-        <v>3105</v>
+        <v>4397</v>
       </c>
       <c r="O4" t="n">
-        <v>57.3314761904762</v>
+        <v>66.583</v>
       </c>
       <c r="P4" t="n">
-        <v>5.43260979728826</v>
+        <v>4.70032783052408</v>
       </c>
       <c r="Q4" t="n">
-        <v>10.0456620426931</v>
+        <v>10.0015149709033</v>
       </c>
       <c r="R4" t="n">
-        <v>34.5454545454545</v>
+        <v>35.7894736842105</v>
       </c>
       <c r="S4" t="n">
         <v>0.3</v>
@@ -707,52 +707,52 @@
         <v>3707770</v>
       </c>
       <c r="D5" t="n">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="E5" t="n">
-        <v>60.2481873222828</v>
+        <v>55.4265564192303</v>
       </c>
       <c r="F5" t="n">
-        <v>76038</v>
+        <v>76827</v>
       </c>
       <c r="G5" t="n">
-        <v>1262.07946461947</v>
+        <v>1386.10451313091</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>0.029</v>
+        <v>0.11</v>
       </c>
       <c r="J5" t="n">
-        <v>23078</v>
+        <v>21381</v>
       </c>
       <c r="K5" t="n">
-        <v>48936</v>
+        <v>51088</v>
       </c>
       <c r="L5" t="n">
-        <v>202</v>
+        <v>162</v>
       </c>
       <c r="M5" t="n">
-        <v>722</v>
+        <v>876</v>
       </c>
       <c r="N5" t="n">
-        <v>3185</v>
+        <v>2960</v>
       </c>
       <c r="O5" t="n">
-        <v>36.331875</v>
+        <v>42.7021746031746</v>
       </c>
       <c r="P5" t="n">
-        <v>12.0781722234907</v>
+        <v>12.1891076133896</v>
       </c>
       <c r="Q5" t="n">
-        <v>14.4760317162351</v>
+        <v>14.0619655080493</v>
       </c>
       <c r="R5" t="n">
         <v>30</v>
       </c>
       <c r="S5" t="n">
-        <v>0.373913043478261</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="6">
@@ -764,52 +764,52 @@
       </c>
       <c r="C6"/>
       <c r="D6" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E6" t="n">
-        <v>50.1163080888244</v>
+        <v>49.0416132262602</v>
       </c>
       <c r="F6" t="n">
-        <v>74082</v>
+        <v>71590</v>
       </c>
       <c r="G6" t="n">
-        <v>1478.2014642559</v>
+        <v>1459.78069011942</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0.077</v>
+        <v>0.25</v>
       </c>
       <c r="J6" t="n">
-        <v>69398</v>
+        <v>66753</v>
       </c>
       <c r="K6" t="n">
-        <v>1739</v>
+        <v>1838</v>
       </c>
       <c r="L6" t="n">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="M6" t="n">
-        <v>1118</v>
+        <v>778</v>
       </c>
       <c r="N6" t="n">
-        <v>1434</v>
+        <v>1298</v>
       </c>
       <c r="O6" t="n">
-        <v>78.9984358974359</v>
+        <v>84.0847105263158</v>
       </c>
       <c r="P6" t="n">
-        <v>3.99624121792894</v>
+        <v>4.02069627852412</v>
       </c>
       <c r="Q6" t="n">
-        <v>3.81139831130443</v>
+        <v>2.70049621750537</v>
       </c>
       <c r="R6" t="n">
-        <v>28.974358974359</v>
+        <v>29.375</v>
       </c>
       <c r="S6" t="n">
-        <v>0.361538461538462</v>
+        <v>0.365625</v>
       </c>
     </row>
     <row r="7">
@@ -823,16 +823,16 @@
         <v>843010</v>
       </c>
       <c r="D7" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" t="n">
-        <v>155.013984349669</v>
+        <v>155.182033671545</v>
       </c>
       <c r="F7" t="n">
-        <v>8997</v>
+        <v>9011</v>
       </c>
       <c r="G7" t="n">
-        <v>58.0399248348152</v>
+        <v>58.067289020535</v>
       </c>
       <c r="H7" t="n">
         <v>1</v>
@@ -841,34 +841,34 @@
         <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>8873</v>
+        <v>8759</v>
       </c>
       <c r="K7" t="n">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="L7" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="M7" t="n">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="N7" t="n">
-        <v>279</v>
+        <v>215</v>
       </c>
       <c r="O7" t="n">
-        <v>55.3237142857143</v>
+        <v>62.2262857142857</v>
       </c>
       <c r="P7" t="n">
-        <v>6.8900563213605</v>
+        <v>11.0061003514899</v>
       </c>
       <c r="Q7" t="n">
-        <v>4.60492319253846</v>
-      </c>
-      <c r="R7" t="n">
-        <v>30</v>
-      </c>
-      <c r="S7" t="n">
-        <v>0.342857142857143</v>
+        <v>5.11730037213777</v>
+      </c>
+      <c r="R7" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S7" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="8">
@@ -882,16 +882,16 @@
         <v>413584</v>
       </c>
       <c r="D8" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E8" t="n">
-        <v>163.018378976147</v>
+        <v>150.568236356283</v>
       </c>
       <c r="F8" t="n">
-        <v>24678</v>
+        <v>17483</v>
       </c>
       <c r="G8" t="n">
-        <v>151.381704044615</v>
+        <v>116.113467375886</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
@@ -900,34 +900,34 @@
         <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>15603</v>
+        <v>9871</v>
       </c>
       <c r="K8" t="n">
-        <v>8460</v>
+        <v>6032</v>
       </c>
       <c r="L8" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M8" t="n">
-        <v>29</v>
+        <v>110</v>
       </c>
       <c r="N8" t="n">
-        <v>668</v>
+        <v>1262</v>
       </c>
       <c r="O8" t="n">
-        <v>73.2828571428571</v>
+        <v>71.8068333333333</v>
       </c>
       <c r="P8" t="n">
-        <v>6.2761254440375</v>
+        <v>6.16883736293026</v>
       </c>
       <c r="Q8" t="n">
-        <v>2.87256612619637</v>
+        <v>6.59066162116396</v>
       </c>
       <c r="R8" t="n">
-        <v>62.5</v>
+        <v>58</v>
       </c>
       <c r="S8" t="n">
-        <v>0.4375</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="9">
@@ -944,13 +944,13 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>194.534577199069</v>
+        <v>179.105185543933</v>
       </c>
       <c r="F9" t="n">
-        <v>24203</v>
+        <v>20205</v>
       </c>
       <c r="G9" t="n">
-        <v>124.414900160566</v>
+        <v>112.810804101726</v>
       </c>
       <c r="H9" t="n">
         <v>1</v>
@@ -959,34 +959,34 @@
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>13347</v>
+        <v>8866</v>
       </c>
       <c r="K9" t="n">
-        <v>10237</v>
+        <v>9730</v>
       </c>
       <c r="L9" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M9" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="N9" t="n">
-        <v>640</v>
+        <v>1310</v>
       </c>
       <c r="O9" t="n">
-        <v>55.8873333333333</v>
+        <v>65.7231111111111</v>
       </c>
       <c r="P9" t="n">
-        <v>5.49989387501395</v>
+        <v>8.3655822976522</v>
       </c>
       <c r="Q9" t="n">
-        <v>3.66226404603994</v>
+        <v>5.49319235766674</v>
       </c>
       <c r="R9" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S9" t="n">
-        <v>0.47</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10">
@@ -998,46 +998,46 @@
       </c>
       <c r="C10"/>
       <c r="D10" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E10" t="n">
-        <v>41.168584416499</v>
+        <v>41.167605010108</v>
       </c>
       <c r="F10" t="n">
-        <v>34103</v>
+        <v>33868</v>
       </c>
       <c r="G10" t="n">
-        <v>828.37436563237</v>
+        <v>822.685701334441</v>
       </c>
       <c r="H10" t="n">
         <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>0.033</v>
+        <v>0.062</v>
       </c>
       <c r="J10" t="n">
-        <v>30175</v>
+        <v>29237</v>
       </c>
       <c r="K10" t="n">
-        <v>1646</v>
+        <v>1493</v>
       </c>
       <c r="L10" t="n">
-        <v>312</v>
+        <v>142</v>
       </c>
       <c r="M10" t="n">
-        <v>647</v>
+        <v>862</v>
       </c>
       <c r="N10" t="n">
-        <v>778</v>
+        <v>1384</v>
       </c>
       <c r="O10" t="n">
-        <v>55.9028571428571</v>
+        <v>67.3829333333333</v>
       </c>
       <c r="P10" t="n">
-        <v>8.22610629400256</v>
+        <v>6.85952029905608</v>
       </c>
       <c r="Q10" t="n">
-        <v>9.60852285055576</v>
+        <v>8.30876749341512</v>
       </c>
       <c r="R10" t="n">
         <v>20</v>
@@ -1057,49 +1057,49 @@
         <v>17240</v>
       </c>
       <c r="D11" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E11" t="n">
-        <v>317.643922321843</v>
+        <v>315.918408936201</v>
       </c>
       <c r="F11" t="n">
-        <v>18344</v>
+        <v>18434</v>
       </c>
       <c r="G11" t="n">
-        <v>57.7501998650348</v>
+        <v>58.3505091142781</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0.9</v>
+        <v>0.91</v>
       </c>
       <c r="J11" t="n">
-        <v>16774</v>
+        <v>16302</v>
       </c>
       <c r="K11" t="n">
-        <v>414</v>
+        <v>424</v>
       </c>
       <c r="L11" t="n">
-        <v>86</v>
+        <v>9</v>
       </c>
       <c r="M11" t="n">
-        <v>167</v>
+        <v>120</v>
       </c>
       <c r="N11" t="n">
-        <v>7453</v>
+        <v>8255</v>
       </c>
       <c r="O11" t="n">
-        <v>76.896</v>
+        <v>85.7849</v>
       </c>
       <c r="P11" t="n">
-        <v>3.48799084402061</v>
+        <v>3.69977641559955</v>
       </c>
       <c r="Q11" t="n">
-        <v>3.28359556469144</v>
+        <v>3.38793267483305</v>
       </c>
       <c r="R11" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="S11" t="n">
         <v>0.2</v>

</xml_diff>